<commit_message>
hotfix + finally compiled
</commit_message>
<xml_diff>
--- a/BFD_report.xlsx
+++ b/BFD_report.xlsx
@@ -1197,7 +1197,7 @@
         <v>10.0</v>
       </c>
       <c r="D2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -1211,7 +1211,7 @@
         <v>10.0</v>
       </c>
       <c r="D3" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -1225,7 +1225,7 @@
         <v>10.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -1239,7 +1239,7 @@
         <v>10.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -1253,7 +1253,7 @@
         <v>10.0</v>
       </c>
       <c r="D6" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -1267,7 +1267,7 @@
         <v>10.0</v>
       </c>
       <c r="D7" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -1281,7 +1281,7 @@
         <v>10.0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -1295,7 +1295,7 @@
         <v>10.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -1309,7 +1309,7 @@
         <v>10.0</v>
       </c>
       <c r="D10" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -1323,7 +1323,7 @@
         <v>10.0</v>
       </c>
       <c r="D11" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -1337,7 +1337,7 @@
         <v>10.0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -1351,7 +1351,7 @@
         <v>10.0</v>
       </c>
       <c r="D13" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -1365,7 +1365,7 @@
         <v>10.0</v>
       </c>
       <c r="D14" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -1379,7 +1379,7 @@
         <v>10.0</v>
       </c>
       <c r="D15" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16">
@@ -1393,7 +1393,7 @@
         <v>10.0</v>
       </c>
       <c r="D16" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -1407,7 +1407,7 @@
         <v>10.0</v>
       </c>
       <c r="D17" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -1421,7 +1421,7 @@
         <v>10.0</v>
       </c>
       <c r="D18" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
@@ -1435,7 +1435,7 @@
         <v>10.0</v>
       </c>
       <c r="D19" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -1449,7 +1449,7 @@
         <v>10.0</v>
       </c>
       <c r="D20" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
@@ -1463,7 +1463,7 @@
         <v>10.0</v>
       </c>
       <c r="D21" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
@@ -1477,7 +1477,7 @@
         <v>10.0</v>
       </c>
       <c r="D22" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23">
@@ -1491,7 +1491,7 @@
         <v>10.0</v>
       </c>
       <c r="D23" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24">
@@ -1505,7 +1505,7 @@
         <v>10.0</v>
       </c>
       <c r="D24" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
@@ -1519,7 +1519,7 @@
         <v>10.0</v>
       </c>
       <c r="D25" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
@@ -1533,7 +1533,7 @@
         <v>10.0</v>
       </c>
       <c r="D26" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27">
@@ -1547,7 +1547,7 @@
         <v>10.0</v>
       </c>
       <c r="D27" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
@@ -1561,7 +1561,7 @@
         <v>10.0</v>
       </c>
       <c r="D28" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
@@ -1575,7 +1575,7 @@
         <v>10.0</v>
       </c>
       <c r="D29" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
@@ -1589,7 +1589,7 @@
         <v>10.0</v>
       </c>
       <c r="D30" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
@@ -1603,7 +1603,7 @@
         <v>10.0</v>
       </c>
       <c r="D31" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
@@ -1617,7 +1617,7 @@
         <v>10.0</v>
       </c>
       <c r="D32" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33">
@@ -1631,7 +1631,7 @@
         <v>10.0</v>
       </c>
       <c r="D33" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
@@ -1645,7 +1645,7 @@
         <v>10.0</v>
       </c>
       <c r="D34" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35">
@@ -1659,7 +1659,7 @@
         <v>9.0</v>
       </c>
       <c r="D35" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.0</v>
       </c>
       <c r="D36" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
@@ -1684,7 +1684,7 @@
         <v>9.0</v>
       </c>
       <c r="D37" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38">
@@ -1695,7 +1695,7 @@
         <v>1.0</v>
       </c>
       <c r="D38" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
@@ -1709,7 +1709,7 @@
         <v>9.0</v>
       </c>
       <c r="D39" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40">
@@ -1720,7 +1720,7 @@
         <v>1.0</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -1734,7 +1734,7 @@
         <v>9.0</v>
       </c>
       <c r="D41" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
@@ -1745,7 +1745,7 @@
         <v>1.0</v>
       </c>
       <c r="D42" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -1759,7 +1759,7 @@
         <v>9.0</v>
       </c>
       <c r="D43" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44">
@@ -1770,7 +1770,7 @@
         <v>1.0</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45">
@@ -1784,7 +1784,7 @@
         <v>9.0</v>
       </c>
       <c r="D45" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -1795,7 +1795,7 @@
         <v>1.0</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -1809,7 +1809,7 @@
         <v>9.0</v>
       </c>
       <c r="D47" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
@@ -1820,7 +1820,7 @@
         <v>1.0</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="49">
@@ -1834,7 +1834,7 @@
         <v>9.0</v>
       </c>
       <c r="D49" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="50">
@@ -1845,7 +1845,7 @@
         <v>1.0</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
@@ -1859,7 +1859,7 @@
         <v>9.0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
@@ -1870,7 +1870,7 @@
         <v>1.0</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="53">
@@ -1884,7 +1884,7 @@
         <v>9.0</v>
       </c>
       <c r="D53" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="54">
@@ -1895,7 +1895,7 @@
         <v>1.0</v>
       </c>
       <c r="D54" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="55">
@@ -1909,7 +1909,7 @@
         <v>9.0</v>
       </c>
       <c r="D55" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="56">
@@ -1920,7 +1920,7 @@
         <v>1.0</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="57">
@@ -1934,7 +1934,7 @@
         <v>9.0</v>
       </c>
       <c r="D57" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="58">
@@ -1945,7 +1945,7 @@
         <v>1.0</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="59">
@@ -1959,7 +1959,7 @@
         <v>9.0</v>
       </c>
       <c r="D59" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="60">
@@ -1970,7 +1970,7 @@
         <v>1.0</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="61">
@@ -1984,7 +1984,7 @@
         <v>9.0</v>
       </c>
       <c r="D61" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="62">
@@ -1995,7 +1995,7 @@
         <v>1.0</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="63">
@@ -2009,7 +2009,7 @@
         <v>9.0</v>
       </c>
       <c r="D63" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="64">
@@ -2020,7 +2020,7 @@
         <v>1.0</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="65">
@@ -2034,7 +2034,7 @@
         <v>9.0</v>
       </c>
       <c r="D65" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="66">
@@ -2045,7 +2045,7 @@
         <v>1.0</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="67">
@@ -2059,7 +2059,7 @@
         <v>9.0</v>
       </c>
       <c r="D67" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="68">
@@ -2070,7 +2070,7 @@
         <v>1.0</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="69">
@@ -2084,7 +2084,7 @@
         <v>9.0</v>
       </c>
       <c r="D69" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="70">
@@ -2095,7 +2095,7 @@
         <v>1.0</v>
       </c>
       <c r="D70" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="71">
@@ -2109,7 +2109,7 @@
         <v>9.0</v>
       </c>
       <c r="D71" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="72">
@@ -2120,7 +2120,7 @@
         <v>1.0</v>
       </c>
       <c r="D72" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="73">
@@ -2134,7 +2134,7 @@
         <v>9.0</v>
       </c>
       <c r="D73" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="74">
@@ -2145,7 +2145,7 @@
         <v>1.0</v>
       </c>
       <c r="D74" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="75">
@@ -2159,7 +2159,7 @@
         <v>9.0</v>
       </c>
       <c r="D75" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="76">
@@ -2170,7 +2170,7 @@
         <v>1.0</v>
       </c>
       <c r="D76" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="77">
@@ -2184,7 +2184,7 @@
         <v>9.0</v>
       </c>
       <c r="D77" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="78">
@@ -2195,7 +2195,7 @@
         <v>1.0</v>
       </c>
       <c r="D78" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="79">
@@ -2209,7 +2209,7 @@
         <v>9.0</v>
       </c>
       <c r="D79" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="80">
@@ -2220,7 +2220,7 @@
         <v>1.0</v>
       </c>
       <c r="D80" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="81">
@@ -2234,7 +2234,7 @@
         <v>9.0</v>
       </c>
       <c r="D81" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="82">
@@ -2245,7 +2245,7 @@
         <v>1.0</v>
       </c>
       <c r="D82" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="83">
@@ -2259,7 +2259,7 @@
         <v>9.0</v>
       </c>
       <c r="D83" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="84">
@@ -2270,7 +2270,7 @@
         <v>1.0</v>
       </c>
       <c r="D84" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="85">
@@ -2284,7 +2284,7 @@
         <v>9.0</v>
       </c>
       <c r="D85" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="86">
@@ -2295,7 +2295,7 @@
         <v>1.0</v>
       </c>
       <c r="D86" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="87">
@@ -2309,7 +2309,7 @@
         <v>9.0</v>
       </c>
       <c r="D87" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="88">
@@ -2320,7 +2320,7 @@
         <v>1.0</v>
       </c>
       <c r="D88" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="89">
@@ -2334,7 +2334,7 @@
         <v>9.0</v>
       </c>
       <c r="D89" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
@@ -2345,7 +2345,7 @@
         <v>1.0</v>
       </c>
       <c r="D90" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="91">
@@ -2359,7 +2359,7 @@
         <v>9.0</v>
       </c>
       <c r="D91" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="92">
@@ -2370,7 +2370,7 @@
         <v>1.0</v>
       </c>
       <c r="D92" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="93">
@@ -2384,7 +2384,7 @@
         <v>9.0</v>
       </c>
       <c r="D93" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="94">
@@ -2395,7 +2395,7 @@
         <v>1.0</v>
       </c>
       <c r="D94" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="95">
@@ -2409,7 +2409,7 @@
         <v>9.0</v>
       </c>
       <c r="D95" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="96">
@@ -2420,7 +2420,7 @@
         <v>1.0</v>
       </c>
       <c r="D96" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="97">
@@ -2434,7 +2434,7 @@
         <v>9.0</v>
       </c>
       <c r="D97" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="98">
@@ -2445,7 +2445,7 @@
         <v>1.0</v>
       </c>
       <c r="D98" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="99">
@@ -2459,7 +2459,7 @@
         <v>9.0</v>
       </c>
       <c r="D99" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="100">
@@ -2470,7 +2470,7 @@
         <v>1.0</v>
       </c>
       <c r="D100" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="101">
@@ -2484,7 +2484,7 @@
         <v>9.0</v>
       </c>
       <c r="D101" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="102">
@@ -2495,7 +2495,7 @@
         <v>1.0</v>
       </c>
       <c r="D102" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="103">
@@ -2509,7 +2509,7 @@
         <v>9.0</v>
       </c>
       <c r="D103" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="104">
@@ -2520,7 +2520,7 @@
         <v>1.0</v>
       </c>
       <c r="D104" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="105">
@@ -2534,7 +2534,7 @@
         <v>9.0</v>
       </c>
       <c r="D105" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="106">
@@ -2545,7 +2545,7 @@
         <v>1.0</v>
       </c>
       <c r="D106" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="107">
@@ -2559,7 +2559,7 @@
         <v>9.0</v>
       </c>
       <c r="D107" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="108">
@@ -2570,7 +2570,7 @@
         <v>1.0</v>
       </c>
       <c r="D108" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="109">
@@ -2584,7 +2584,7 @@
         <v>9.0</v>
       </c>
       <c r="D109" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="110">
@@ -2595,7 +2595,7 @@
         <v>1.0</v>
       </c>
       <c r="D110" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="111">
@@ -2609,7 +2609,7 @@
         <v>9.0</v>
       </c>
       <c r="D111" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="112">
@@ -2620,7 +2620,7 @@
         <v>1.0</v>
       </c>
       <c r="D112" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="113">
@@ -2634,7 +2634,7 @@
         <v>9.0</v>
       </c>
       <c r="D113" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="114">
@@ -2645,7 +2645,7 @@
         <v>1.0</v>
       </c>
       <c r="D114" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="115">
@@ -2659,7 +2659,7 @@
         <v>9.0</v>
       </c>
       <c r="D115" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="116">
@@ -2670,7 +2670,7 @@
         <v>1.0</v>
       </c>
       <c r="D116" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="117">
@@ -2684,7 +2684,7 @@
         <v>9.0</v>
       </c>
       <c r="D117" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="118">
@@ -2695,7 +2695,7 @@
         <v>1.0</v>
       </c>
       <c r="D118" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="119">
@@ -2709,7 +2709,7 @@
         <v>9.0</v>
       </c>
       <c r="D119" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="120">
@@ -2720,7 +2720,7 @@
         <v>1.0</v>
       </c>
       <c r="D120" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="121">
@@ -2734,7 +2734,7 @@
         <v>9.0</v>
       </c>
       <c r="D121" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="122">
@@ -2745,7 +2745,7 @@
         <v>1.0</v>
       </c>
       <c r="D122" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="123">
@@ -2759,7 +2759,7 @@
         <v>9.0</v>
       </c>
       <c r="D123" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="124">
@@ -2773,7 +2773,7 @@
         <v>9.0</v>
       </c>
       <c r="D124" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="125">
@@ -2787,7 +2787,7 @@
         <v>9.0</v>
       </c>
       <c r="D125" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="126">
@@ -2801,7 +2801,7 @@
         <v>9.0</v>
       </c>
       <c r="D126" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="127">
@@ -2815,7 +2815,7 @@
         <v>9.0</v>
       </c>
       <c r="D127" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="128">
@@ -2829,7 +2829,7 @@
         <v>9.0</v>
       </c>
       <c r="D128" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="129">
@@ -2843,7 +2843,7 @@
         <v>9.0</v>
       </c>
       <c r="D129" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="130">
@@ -2857,7 +2857,7 @@
         <v>8.0</v>
       </c>
       <c r="D130" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="131">
@@ -2868,7 +2868,7 @@
         <v>2.0</v>
       </c>
       <c r="D131" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="132">
@@ -2882,7 +2882,7 @@
         <v>8.0</v>
       </c>
       <c r="D132" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="133">
@@ -2893,7 +2893,7 @@
         <v>2.0</v>
       </c>
       <c r="D133" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="134">
@@ -2907,7 +2907,7 @@
         <v>8.0</v>
       </c>
       <c r="D134" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="135">
@@ -2918,7 +2918,7 @@
         <v>2.0</v>
       </c>
       <c r="D135" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="136">
@@ -2932,7 +2932,7 @@
         <v>8.0</v>
       </c>
       <c r="D136" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="137">
@@ -2943,7 +2943,7 @@
         <v>2.0</v>
       </c>
       <c r="D137" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="138">
@@ -2957,7 +2957,7 @@
         <v>8.0</v>
       </c>
       <c r="D138" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="139">
@@ -2968,7 +2968,7 @@
         <v>2.0</v>
       </c>
       <c r="D139" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="140">
@@ -2982,7 +2982,7 @@
         <v>8.0</v>
       </c>
       <c r="D140" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="141">
@@ -2993,7 +2993,7 @@
         <v>2.0</v>
       </c>
       <c r="D141" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="142">
@@ -3007,7 +3007,7 @@
         <v>8.0</v>
       </c>
       <c r="D142" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="143">
@@ -3018,7 +3018,7 @@
         <v>2.0</v>
       </c>
       <c r="D143" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="144">
@@ -3032,7 +3032,7 @@
         <v>8.0</v>
       </c>
       <c r="D144" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="145">
@@ -3043,7 +3043,7 @@
         <v>2.0</v>
       </c>
       <c r="D145" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="146">
@@ -3057,7 +3057,7 @@
         <v>8.0</v>
       </c>
       <c r="D146" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="147">
@@ -3068,7 +3068,7 @@
         <v>2.0</v>
       </c>
       <c r="D147" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="148">
@@ -3082,7 +3082,7 @@
         <v>8.0</v>
       </c>
       <c r="D148" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="149">
@@ -3093,7 +3093,7 @@
         <v>2.0</v>
       </c>
       <c r="D149" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="150">
@@ -3107,7 +3107,7 @@
         <v>8.0</v>
       </c>
       <c r="D150" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="151">
@@ -3118,7 +3118,7 @@
         <v>2.0</v>
       </c>
       <c r="D151" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="152">
@@ -3132,7 +3132,7 @@
         <v>8.0</v>
       </c>
       <c r="D152" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="153">
@@ -3143,7 +3143,7 @@
         <v>2.0</v>
       </c>
       <c r="D153" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="154">
@@ -3157,7 +3157,7 @@
         <v>8.0</v>
       </c>
       <c r="D154" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="155">
@@ -3168,7 +3168,7 @@
         <v>2.0</v>
       </c>
       <c r="D155" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="156">
@@ -3182,7 +3182,7 @@
         <v>8.0</v>
       </c>
       <c r="D156" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="157">
@@ -3193,7 +3193,7 @@
         <v>2.0</v>
       </c>
       <c r="D157" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="158">
@@ -3207,7 +3207,7 @@
         <v>8.0</v>
       </c>
       <c r="D158" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="159">
@@ -3218,7 +3218,7 @@
         <v>2.0</v>
       </c>
       <c r="D159" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="160">
@@ -3232,7 +3232,7 @@
         <v>8.0</v>
       </c>
       <c r="D160" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="161">
@@ -3243,7 +3243,7 @@
         <v>2.0</v>
       </c>
       <c r="D161" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="162">
@@ -3257,7 +3257,7 @@
         <v>8.0</v>
       </c>
       <c r="D162" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="163">
@@ -3268,7 +3268,7 @@
         <v>2.0</v>
       </c>
       <c r="D163" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="164">
@@ -3282,7 +3282,7 @@
         <v>8.0</v>
       </c>
       <c r="D164" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="165">
@@ -3293,7 +3293,7 @@
         <v>2.0</v>
       </c>
       <c r="D165" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="166">
@@ -3307,7 +3307,7 @@
         <v>8.0</v>
       </c>
       <c r="D166" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="167">
@@ -3318,7 +3318,7 @@
         <v>2.0</v>
       </c>
       <c r="D167" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="168">
@@ -3332,7 +3332,7 @@
         <v>8.0</v>
       </c>
       <c r="D168" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="169">
@@ -3343,7 +3343,7 @@
         <v>2.0</v>
       </c>
       <c r="D169" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="170">
@@ -3357,7 +3357,7 @@
         <v>8.0</v>
       </c>
       <c r="D170" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="171">
@@ -3368,7 +3368,7 @@
         <v>2.0</v>
       </c>
       <c r="D171" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="172">
@@ -3382,7 +3382,7 @@
         <v>8.0</v>
       </c>
       <c r="D172" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="173">
@@ -3393,7 +3393,7 @@
         <v>2.0</v>
       </c>
       <c r="D173" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="174">
@@ -3407,7 +3407,7 @@
         <v>8.0</v>
       </c>
       <c r="D174" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="175">
@@ -3418,7 +3418,7 @@
         <v>2.0</v>
       </c>
       <c r="D175" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="176">
@@ -3432,7 +3432,7 @@
         <v>8.0</v>
       </c>
       <c r="D176" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="177">
@@ -3443,7 +3443,7 @@
         <v>2.0</v>
       </c>
       <c r="D177" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="178">
@@ -3457,7 +3457,7 @@
         <v>8.0</v>
       </c>
       <c r="D178" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="179">
@@ -3468,7 +3468,7 @@
         <v>2.0</v>
       </c>
       <c r="D179" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="180">
@@ -3482,7 +3482,7 @@
         <v>8.0</v>
       </c>
       <c r="D180" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="181">
@@ -3493,7 +3493,7 @@
         <v>2.0</v>
       </c>
       <c r="D181" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="182">
@@ -3507,7 +3507,7 @@
         <v>8.0</v>
       </c>
       <c r="D182" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="183">
@@ -3518,7 +3518,7 @@
         <v>2.0</v>
       </c>
       <c r="D183" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="184">
@@ -3532,7 +3532,7 @@
         <v>8.0</v>
       </c>
       <c r="D184" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="185">
@@ -3543,7 +3543,7 @@
         <v>2.0</v>
       </c>
       <c r="D185" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="186">
@@ -3557,7 +3557,7 @@
         <v>8.0</v>
       </c>
       <c r="D186" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="187">
@@ -3568,7 +3568,7 @@
         <v>2.0</v>
       </c>
       <c r="D187" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="188">
@@ -3582,7 +3582,7 @@
         <v>8.0</v>
       </c>
       <c r="D188" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="189">
@@ -3593,7 +3593,7 @@
         <v>2.0</v>
       </c>
       <c r="D189" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="190">
@@ -3607,7 +3607,7 @@
         <v>8.0</v>
       </c>
       <c r="D190" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="191">
@@ -3618,7 +3618,7 @@
         <v>2.0</v>
       </c>
       <c r="D191" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="192">
@@ -3632,7 +3632,7 @@
         <v>8.0</v>
       </c>
       <c r="D192" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="193">
@@ -3643,7 +3643,7 @@
         <v>2.0</v>
       </c>
       <c r="D193" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="194">
@@ -3657,7 +3657,7 @@
         <v>8.0</v>
       </c>
       <c r="D194" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="195">
@@ -3668,7 +3668,7 @@
         <v>2.0</v>
       </c>
       <c r="D195" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="196">
@@ -3682,7 +3682,7 @@
         <v>8.0</v>
       </c>
       <c r="D196" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="197">
@@ -3693,7 +3693,7 @@
         <v>2.0</v>
       </c>
       <c r="D197" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="198">
@@ -3707,7 +3707,7 @@
         <v>8.0</v>
       </c>
       <c r="D198" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="199">
@@ -3718,7 +3718,7 @@
         <v>2.0</v>
       </c>
       <c r="D199" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="200">
@@ -3732,7 +3732,7 @@
         <v>8.0</v>
       </c>
       <c r="D200" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="201">
@@ -3743,7 +3743,7 @@
         <v>2.0</v>
       </c>
       <c r="D201" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="202">
@@ -3757,7 +3757,7 @@
         <v>8.0</v>
       </c>
       <c r="D202" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="203">
@@ -3768,7 +3768,7 @@
         <v>2.0</v>
       </c>
       <c r="D203" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="204">
@@ -3782,7 +3782,7 @@
         <v>8.0</v>
       </c>
       <c r="D204" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="205">
@@ -3793,7 +3793,7 @@
         <v>2.0</v>
       </c>
       <c r="D205" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="206">
@@ -3807,7 +3807,7 @@
         <v>8.0</v>
       </c>
       <c r="D206" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="207">
@@ -3818,7 +3818,7 @@
         <v>2.0</v>
       </c>
       <c r="D207" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="208">
@@ -3832,7 +3832,7 @@
         <v>8.0</v>
       </c>
       <c r="D208" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="209">
@@ -3843,7 +3843,7 @@
         <v>2.0</v>
       </c>
       <c r="D209" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="210">
@@ -3857,7 +3857,7 @@
         <v>8.0</v>
       </c>
       <c r="D210" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="211">
@@ -3868,7 +3868,7 @@
         <v>2.0</v>
       </c>
       <c r="D211" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="212">
@@ -3882,7 +3882,7 @@
         <v>8.0</v>
       </c>
       <c r="D212" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="213">
@@ -3893,7 +3893,7 @@
         <v>2.0</v>
       </c>
       <c r="D213" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="214">
@@ -3907,7 +3907,7 @@
         <v>8.0</v>
       </c>
       <c r="D214" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="215">
@@ -3918,7 +3918,7 @@
         <v>2.0</v>
       </c>
       <c r="D215" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="216">
@@ -3932,7 +3932,7 @@
         <v>8.0</v>
       </c>
       <c r="D216" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="217">
@@ -3943,7 +3943,7 @@
         <v>2.0</v>
       </c>
       <c r="D217" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="218">
@@ -3957,7 +3957,7 @@
         <v>8.0</v>
       </c>
       <c r="D218" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="219">
@@ -3968,7 +3968,7 @@
         <v>2.0</v>
       </c>
       <c r="D219" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="220">
@@ -3982,7 +3982,7 @@
         <v>8.0</v>
       </c>
       <c r="D220" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="221">
@@ -3993,7 +3993,7 @@
         <v>2.0</v>
       </c>
       <c r="D221" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="222">
@@ -4007,7 +4007,7 @@
         <v>8.0</v>
       </c>
       <c r="D222" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="223">
@@ -4018,7 +4018,7 @@
         <v>2.0</v>
       </c>
       <c r="D223" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="224">
@@ -4032,7 +4032,7 @@
         <v>8.0</v>
       </c>
       <c r="D224" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="225">
@@ -4043,7 +4043,7 @@
         <v>2.0</v>
       </c>
       <c r="D225" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="226">
@@ -4057,7 +4057,7 @@
         <v>8.0</v>
       </c>
       <c r="D226" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="227">
@@ -4068,7 +4068,7 @@
         <v>2.0</v>
       </c>
       <c r="D227" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="228">
@@ -4082,7 +4082,7 @@
         <v>8.0</v>
       </c>
       <c r="D228" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="229">
@@ -4093,7 +4093,7 @@
         <v>2.0</v>
       </c>
       <c r="D229" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="230">
@@ -4107,7 +4107,7 @@
         <v>8.0</v>
       </c>
       <c r="D230" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="231">
@@ -4118,7 +4118,7 @@
         <v>2.0</v>
       </c>
       <c r="D231" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="232">
@@ -4132,7 +4132,7 @@
         <v>8.0</v>
       </c>
       <c r="D232" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="233">
@@ -4143,7 +4143,7 @@
         <v>2.0</v>
       </c>
       <c r="D233" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="234">
@@ -4157,7 +4157,7 @@
         <v>8.0</v>
       </c>
       <c r="D234" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="235">
@@ -4171,7 +4171,7 @@
         <v>8.0</v>
       </c>
       <c r="D235" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="236">
@@ -4185,7 +4185,7 @@
         <v>8.0</v>
       </c>
       <c r="D236" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="237">
@@ -4199,7 +4199,7 @@
         <v>8.0</v>
       </c>
       <c r="D237" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="238">
@@ -4213,7 +4213,7 @@
         <v>8.0</v>
       </c>
       <c r="D238" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="239">
@@ -4227,7 +4227,7 @@
         <v>8.0</v>
       </c>
       <c r="D239" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="240">
@@ -4241,7 +4241,7 @@
         <v>8.0</v>
       </c>
       <c r="D240" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="241">
@@ -4255,7 +4255,7 @@
         <v>8.0</v>
       </c>
       <c r="D241" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="242">
@@ -4269,7 +4269,7 @@
         <v>8.0</v>
       </c>
       <c r="D242" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="243">
@@ -4283,7 +4283,7 @@
         <v>7.0</v>
       </c>
       <c r="D243" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="244">
@@ -4294,7 +4294,7 @@
         <v>3.0</v>
       </c>
       <c r="D244" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="245">
@@ -4308,7 +4308,7 @@
         <v>7.0</v>
       </c>
       <c r="D245" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="246">
@@ -4319,7 +4319,7 @@
         <v>3.0</v>
       </c>
       <c r="D246" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="247">
@@ -4333,7 +4333,7 @@
         <v>7.0</v>
       </c>
       <c r="D247" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="248">
@@ -4344,7 +4344,7 @@
         <v>3.0</v>
       </c>
       <c r="D248" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="249">
@@ -4358,7 +4358,7 @@
         <v>7.0</v>
       </c>
       <c r="D249" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="250">
@@ -4369,7 +4369,7 @@
         <v>3.0</v>
       </c>
       <c r="D250" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="251">
@@ -4383,7 +4383,7 @@
         <v>7.0</v>
       </c>
       <c r="D251" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="252">
@@ -4394,7 +4394,7 @@
         <v>3.0</v>
       </c>
       <c r="D252" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="253">
@@ -4408,7 +4408,7 @@
         <v>7.0</v>
       </c>
       <c r="D253" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="254">
@@ -4419,7 +4419,7 @@
         <v>3.0</v>
       </c>
       <c r="D254" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="255">
@@ -4433,7 +4433,7 @@
         <v>7.0</v>
       </c>
       <c r="D255" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="256">
@@ -4444,7 +4444,7 @@
         <v>3.0</v>
       </c>
       <c r="D256" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="257">
@@ -4458,7 +4458,7 @@
         <v>7.0</v>
       </c>
       <c r="D257" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="258">
@@ -4469,7 +4469,7 @@
         <v>3.0</v>
       </c>
       <c r="D258" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="259">
@@ -4483,7 +4483,7 @@
         <v>7.0</v>
       </c>
       <c r="D259" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="260">
@@ -4494,7 +4494,7 @@
         <v>3.0</v>
       </c>
       <c r="D260" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="261">
@@ -4508,7 +4508,7 @@
         <v>7.0</v>
       </c>
       <c r="D261" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="262">
@@ -4519,7 +4519,7 @@
         <v>3.0</v>
       </c>
       <c r="D262" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="263">
@@ -4533,7 +4533,7 @@
         <v>7.0</v>
       </c>
       <c r="D263" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="264">
@@ -4544,7 +4544,7 @@
         <v>3.0</v>
       </c>
       <c r="D264" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="265">
@@ -4558,7 +4558,7 @@
         <v>7.0</v>
       </c>
       <c r="D265" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="266">
@@ -4569,7 +4569,7 @@
         <v>3.0</v>
       </c>
       <c r="D266" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="267">
@@ -4583,7 +4583,7 @@
         <v>7.0</v>
       </c>
       <c r="D267" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="268">
@@ -4594,7 +4594,7 @@
         <v>3.0</v>
       </c>
       <c r="D268" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="269">
@@ -4608,7 +4608,7 @@
         <v>7.0</v>
       </c>
       <c r="D269" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="270">
@@ -4619,7 +4619,7 @@
         <v>3.0</v>
       </c>
       <c r="D270" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="271">
@@ -4633,7 +4633,7 @@
         <v>7.0</v>
       </c>
       <c r="D271" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="272">
@@ -4644,7 +4644,7 @@
         <v>3.0</v>
       </c>
       <c r="D272" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="273">
@@ -4658,7 +4658,7 @@
         <v>7.0</v>
       </c>
       <c r="D273" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="274">
@@ -4669,7 +4669,7 @@
         <v>3.0</v>
       </c>
       <c r="D274" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="275">
@@ -4683,7 +4683,7 @@
         <v>7.0</v>
       </c>
       <c r="D275" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="276">
@@ -4694,7 +4694,7 @@
         <v>3.0</v>
       </c>
       <c r="D276" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="277">
@@ -4708,7 +4708,7 @@
         <v>7.0</v>
       </c>
       <c r="D277" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="278">
@@ -4719,7 +4719,7 @@
         <v>3.0</v>
       </c>
       <c r="D278" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="279">
@@ -4733,7 +4733,7 @@
         <v>7.0</v>
       </c>
       <c r="D279" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="280">
@@ -4744,7 +4744,7 @@
         <v>3.0</v>
       </c>
       <c r="D280" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="281">
@@ -4758,7 +4758,7 @@
         <v>7.0</v>
       </c>
       <c r="D281" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="282">
@@ -4769,7 +4769,7 @@
         <v>3.0</v>
       </c>
       <c r="D282" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="283">
@@ -4783,7 +4783,7 @@
         <v>7.0</v>
       </c>
       <c r="D283" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="284">
@@ -4794,7 +4794,7 @@
         <v>3.0</v>
       </c>
       <c r="D284" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="285">
@@ -4808,7 +4808,7 @@
         <v>7.0</v>
       </c>
       <c r="D285" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="286">
@@ -4819,7 +4819,7 @@
         <v>3.0</v>
       </c>
       <c r="D286" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="287">
@@ -4833,7 +4833,7 @@
         <v>7.0</v>
       </c>
       <c r="D287" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="288">
@@ -4844,7 +4844,7 @@
         <v>3.0</v>
       </c>
       <c r="D288" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="289">
@@ -4858,7 +4858,7 @@
         <v>7.0</v>
       </c>
       <c r="D289" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="290">
@@ -4869,7 +4869,7 @@
         <v>3.0</v>
       </c>
       <c r="D290" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="291">
@@ -4883,7 +4883,7 @@
         <v>7.0</v>
       </c>
       <c r="D291" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="292">
@@ -4894,7 +4894,7 @@
         <v>3.0</v>
       </c>
       <c r="D292" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="293">
@@ -4908,7 +4908,7 @@
         <v>7.0</v>
       </c>
       <c r="D293" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="294">
@@ -4919,7 +4919,7 @@
         <v>3.0</v>
       </c>
       <c r="D294" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="295">
@@ -4933,7 +4933,7 @@
         <v>7.0</v>
       </c>
       <c r="D295" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="296">
@@ -4944,7 +4944,7 @@
         <v>3.0</v>
       </c>
       <c r="D296" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="297">
@@ -4958,7 +4958,7 @@
         <v>7.0</v>
       </c>
       <c r="D297" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="298">
@@ -4969,7 +4969,7 @@
         <v>3.0</v>
       </c>
       <c r="D298" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="299">
@@ -4983,7 +4983,7 @@
         <v>7.0</v>
       </c>
       <c r="D299" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="300">
@@ -4994,7 +4994,7 @@
         <v>3.0</v>
       </c>
       <c r="D300" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="301">
@@ -5008,7 +5008,7 @@
         <v>7.0</v>
       </c>
       <c r="D301" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="302">
@@ -5019,7 +5019,7 @@
         <v>3.0</v>
       </c>
       <c r="D302" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="303">
@@ -5033,7 +5033,7 @@
         <v>7.0</v>
       </c>
       <c r="D303" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="304">
@@ -5044,7 +5044,7 @@
         <v>3.0</v>
       </c>
       <c r="D304" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="305">
@@ -5058,7 +5058,7 @@
         <v>6.0</v>
       </c>
       <c r="D305" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="306">
@@ -5069,7 +5069,7 @@
         <v>4.0</v>
       </c>
       <c r="D306" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="307">
@@ -5083,7 +5083,7 @@
         <v>6.0</v>
       </c>
       <c r="D307" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="308">
@@ -5094,7 +5094,7 @@
         <v>4.0</v>
       </c>
       <c r="D308" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="309">
@@ -5108,7 +5108,7 @@
         <v>6.0</v>
       </c>
       <c r="D309" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="310">
@@ -5119,7 +5119,7 @@
         <v>4.0</v>
       </c>
       <c r="D310" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="311">
@@ -5133,7 +5133,7 @@
         <v>6.0</v>
       </c>
       <c r="D311" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="312">
@@ -5144,7 +5144,7 @@
         <v>4.0</v>
       </c>
       <c r="D312" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="313">
@@ -5158,7 +5158,7 @@
         <v>6.0</v>
       </c>
       <c r="D313" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="314">
@@ -5169,7 +5169,7 @@
         <v>4.0</v>
       </c>
       <c r="D314" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="315">
@@ -5183,7 +5183,7 @@
         <v>6.0</v>
       </c>
       <c r="D315" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="316">
@@ -5194,7 +5194,7 @@
         <v>4.0</v>
       </c>
       <c r="D316" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="317">
@@ -5208,7 +5208,7 @@
         <v>6.0</v>
       </c>
       <c r="D317" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="318">
@@ -5219,7 +5219,7 @@
         <v>4.0</v>
       </c>
       <c r="D318" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="319">
@@ -5233,7 +5233,7 @@
         <v>6.0</v>
       </c>
       <c r="D319" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="320">
@@ -5244,7 +5244,7 @@
         <v>4.0</v>
       </c>
       <c r="D320" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="321">
@@ -5258,7 +5258,7 @@
         <v>6.0</v>
       </c>
       <c r="D321" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="322">
@@ -5269,7 +5269,7 @@
         <v>4.0</v>
       </c>
       <c r="D322" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="323">
@@ -5283,7 +5283,7 @@
         <v>6.0</v>
       </c>
       <c r="D323" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="324">
@@ -5294,7 +5294,7 @@
         <v>4.0</v>
       </c>
       <c r="D324" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="325">
@@ -5308,7 +5308,7 @@
         <v>6.0</v>
       </c>
       <c r="D325" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="326">
@@ -5319,7 +5319,7 @@
         <v>4.0</v>
       </c>
       <c r="D326" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="327">
@@ -5333,7 +5333,7 @@
         <v>6.0</v>
       </c>
       <c r="D327" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="328">
@@ -5344,7 +5344,7 @@
         <v>4.0</v>
       </c>
       <c r="D328" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="329">
@@ -5358,7 +5358,7 @@
         <v>6.0</v>
       </c>
       <c r="D329" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="330">
@@ -5369,7 +5369,7 @@
         <v>4.0</v>
       </c>
       <c r="D330" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="331">
@@ -5383,7 +5383,7 @@
         <v>6.0</v>
       </c>
       <c r="D331" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="332">
@@ -5394,7 +5394,7 @@
         <v>4.0</v>
       </c>
       <c r="D332" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="333">
@@ -5408,7 +5408,7 @@
         <v>6.0</v>
       </c>
       <c r="D333" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="334">
@@ -5419,7 +5419,7 @@
         <v>4.0</v>
       </c>
       <c r="D334" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="335">
@@ -5433,7 +5433,7 @@
         <v>6.0</v>
       </c>
       <c r="D335" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="336">
@@ -5444,7 +5444,7 @@
         <v>4.0</v>
       </c>
       <c r="D336" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="337">
@@ -5458,7 +5458,7 @@
         <v>6.0</v>
       </c>
       <c r="D337" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="338">
@@ -5469,7 +5469,7 @@
         <v>4.0</v>
       </c>
       <c r="D338" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="339">
@@ -5483,7 +5483,7 @@
         <v>6.0</v>
       </c>
       <c r="D339" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="340">
@@ -5494,7 +5494,7 @@
         <v>4.0</v>
       </c>
       <c r="D340" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="341">
@@ -5508,7 +5508,7 @@
         <v>6.0</v>
       </c>
       <c r="D341" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="342">
@@ -5519,7 +5519,7 @@
         <v>4.0</v>
       </c>
       <c r="D342" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="343">
@@ -5533,7 +5533,7 @@
         <v>6.0</v>
       </c>
       <c r="D343" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="344">
@@ -5544,7 +5544,7 @@
         <v>4.0</v>
       </c>
       <c r="D344" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="345">
@@ -5558,7 +5558,7 @@
         <v>6.0</v>
       </c>
       <c r="D345" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="346">
@@ -5569,7 +5569,7 @@
         <v>4.0</v>
       </c>
       <c r="D346" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="347">
@@ -5583,7 +5583,7 @@
         <v>6.0</v>
       </c>
       <c r="D347" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="348">
@@ -5594,7 +5594,7 @@
         <v>4.0</v>
       </c>
       <c r="D348" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="349">
@@ -5608,7 +5608,7 @@
         <v>6.0</v>
       </c>
       <c r="D349" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="350">
@@ -5619,7 +5619,7 @@
         <v>4.0</v>
       </c>
       <c r="D350" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="351">
@@ -5633,7 +5633,7 @@
         <v>6.0</v>
       </c>
       <c r="D351" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="352">
@@ -5644,7 +5644,7 @@
         <v>4.0</v>
       </c>
       <c r="D352" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="353">
@@ -5658,7 +5658,7 @@
         <v>6.0</v>
       </c>
       <c r="D353" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="354">
@@ -5669,7 +5669,7 @@
         <v>4.0</v>
       </c>
       <c r="D354" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="355">
@@ -5683,7 +5683,7 @@
         <v>6.0</v>
       </c>
       <c r="D355" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="356">
@@ -5694,7 +5694,7 @@
         <v>4.0</v>
       </c>
       <c r="D356" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="357">
@@ -5708,7 +5708,7 @@
         <v>6.0</v>
       </c>
       <c r="D357" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="358">
@@ -5719,7 +5719,7 @@
         <v>4.0</v>
       </c>
       <c r="D358" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="359">
@@ -5733,7 +5733,7 @@
         <v>6.0</v>
       </c>
       <c r="D359" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="360">
@@ -5744,7 +5744,7 @@
         <v>4.0</v>
       </c>
       <c r="D360" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="361">
@@ -5758,7 +5758,7 @@
         <v>6.0</v>
       </c>
       <c r="D361" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="362">
@@ -5769,7 +5769,7 @@
         <v>4.0</v>
       </c>
       <c r="D362" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="363">
@@ -5783,7 +5783,7 @@
         <v>6.0</v>
       </c>
       <c r="D363" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="364">
@@ -5794,7 +5794,7 @@
         <v>4.0</v>
       </c>
       <c r="D364" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="365">
@@ -5808,7 +5808,7 @@
         <v>6.0</v>
       </c>
       <c r="D365" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="366">
@@ -5819,7 +5819,7 @@
         <v>4.0</v>
       </c>
       <c r="D366" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="367">
@@ -5833,7 +5833,7 @@
         <v>6.0</v>
       </c>
       <c r="D367" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="368">
@@ -5844,7 +5844,7 @@
         <v>4.0</v>
       </c>
       <c r="D368" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="369">
@@ -5858,7 +5858,7 @@
         <v>6.0</v>
       </c>
       <c r="D369" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="370">
@@ -5869,7 +5869,7 @@
         <v>4.0</v>
       </c>
       <c r="D370" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="371">
@@ -5883,7 +5883,7 @@
         <v>6.0</v>
       </c>
       <c r="D371" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="372">
@@ -5894,7 +5894,7 @@
         <v>4.0</v>
       </c>
       <c r="D372" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="373">
@@ -5908,7 +5908,7 @@
         <v>6.0</v>
       </c>
       <c r="D373" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="374">
@@ -5919,7 +5919,7 @@
         <v>4.0</v>
       </c>
       <c r="D374" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="375">
@@ -5933,7 +5933,7 @@
         <v>6.0</v>
       </c>
       <c r="D375" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="376">
@@ -5944,7 +5944,7 @@
         <v>4.0</v>
       </c>
       <c r="D376" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="377">
@@ -5958,7 +5958,7 @@
         <v>6.0</v>
       </c>
       <c r="D377" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="378">
@@ -5969,7 +5969,7 @@
         <v>4.0</v>
       </c>
       <c r="D378" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="379">
@@ -5983,7 +5983,7 @@
         <v>6.0</v>
       </c>
       <c r="D379" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="380">
@@ -5994,7 +5994,7 @@
         <v>4.0</v>
       </c>
       <c r="D380" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="381">
@@ -6008,7 +6008,7 @@
         <v>6.0</v>
       </c>
       <c r="D381" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="382">
@@ -6019,7 +6019,7 @@
         <v>4.0</v>
       </c>
       <c r="D382" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="383">
@@ -6033,7 +6033,7 @@
         <v>6.0</v>
       </c>
       <c r="D383" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="384">
@@ -6044,7 +6044,7 @@
         <v>4.0</v>
       </c>
       <c r="D384" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="385">
@@ -6058,7 +6058,7 @@
         <v>6.0</v>
       </c>
       <c r="D385" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="386">
@@ -6069,7 +6069,7 @@
         <v>4.0</v>
       </c>
       <c r="D386" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="387">
@@ -6083,7 +6083,7 @@
         <v>6.0</v>
       </c>
       <c r="D387" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="388">
@@ -6094,7 +6094,7 @@
         <v>4.0</v>
       </c>
       <c r="D388" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="389">
@@ -6108,7 +6108,7 @@
         <v>5.0</v>
       </c>
       <c r="D389" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="390">
@@ -6119,7 +6119,7 @@
         <v>5.0</v>
       </c>
       <c r="D390" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="391">
@@ -6133,7 +6133,7 @@
         <v>5.0</v>
       </c>
       <c r="D391" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="392">
@@ -6144,7 +6144,7 @@
         <v>5.0</v>
       </c>
       <c r="D392" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="393">
@@ -6158,7 +6158,7 @@
         <v>5.0</v>
       </c>
       <c r="D393" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="394">
@@ -6169,7 +6169,7 @@
         <v>5.0</v>
       </c>
       <c r="D394" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="395">
@@ -6183,7 +6183,7 @@
         <v>5.0</v>
       </c>
       <c r="D395" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="396">
@@ -6194,7 +6194,7 @@
         <v>5.0</v>
       </c>
       <c r="D396" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="397">
@@ -6208,7 +6208,7 @@
         <v>5.0</v>
       </c>
       <c r="D397" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="398">
@@ -6219,7 +6219,7 @@
         <v>5.0</v>
       </c>
       <c r="D398" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="399">
@@ -6233,7 +6233,7 @@
         <v>5.0</v>
       </c>
       <c r="D399" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="400">
@@ -6244,7 +6244,7 @@
         <v>5.0</v>
       </c>
       <c r="D400" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="401">
@@ -6258,7 +6258,7 @@
         <v>5.0</v>
       </c>
       <c r="D401" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="402">
@@ -6269,7 +6269,7 @@
         <v>5.0</v>
       </c>
       <c r="D402" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="403">
@@ -6283,7 +6283,7 @@
         <v>5.0</v>
       </c>
       <c r="D403" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="404">
@@ -6294,7 +6294,7 @@
         <v>5.0</v>
       </c>
       <c r="D404" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="405">
@@ -6308,7 +6308,7 @@
         <v>5.0</v>
       </c>
       <c r="D405" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="406">
@@ -6319,7 +6319,7 @@
         <v>5.0</v>
       </c>
       <c r="D406" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="407">
@@ -6333,7 +6333,7 @@
         <v>5.0</v>
       </c>
       <c r="D407" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="408">
@@ -6344,7 +6344,7 @@
         <v>5.0</v>
       </c>
       <c r="D408" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="409">
@@ -6358,7 +6358,7 @@
         <v>5.0</v>
       </c>
       <c r="D409" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="410">
@@ -6369,7 +6369,7 @@
         <v>5.0</v>
       </c>
       <c r="D410" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="411">
@@ -6383,7 +6383,7 @@
         <v>5.0</v>
       </c>
       <c r="D411" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="412">
@@ -6394,7 +6394,7 @@
         <v>5.0</v>
       </c>
       <c r="D412" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="413">
@@ -6408,7 +6408,7 @@
         <v>5.0</v>
       </c>
       <c r="D413" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="414">
@@ -6419,7 +6419,7 @@
         <v>5.0</v>
       </c>
       <c r="D414" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="415">
@@ -6433,7 +6433,7 @@
         <v>5.0</v>
       </c>
       <c r="D415" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="416">
@@ -6444,7 +6444,7 @@
         <v>5.0</v>
       </c>
       <c r="D416" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="417">
@@ -6458,7 +6458,7 @@
         <v>5.0</v>
       </c>
       <c r="D417" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="418">
@@ -6469,7 +6469,7 @@
         <v>5.0</v>
       </c>
       <c r="D418" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="419">
@@ -6483,7 +6483,7 @@
         <v>5.0</v>
       </c>
       <c r="D419" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="420">
@@ -6494,7 +6494,7 @@
         <v>5.0</v>
       </c>
       <c r="D420" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="421">
@@ -6508,7 +6508,7 @@
         <v>5.0</v>
       </c>
       <c r="D421" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="422">
@@ -6519,7 +6519,7 @@
         <v>5.0</v>
       </c>
       <c r="D422" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="423">
@@ -6533,7 +6533,7 @@
         <v>5.0</v>
       </c>
       <c r="D423" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="424">
@@ -6544,7 +6544,7 @@
         <v>5.0</v>
       </c>
       <c r="D424" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="425">
@@ -6558,7 +6558,7 @@
         <v>5.0</v>
       </c>
       <c r="D425" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="426">
@@ -6569,7 +6569,7 @@
         <v>5.0</v>
       </c>
       <c r="D426" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="427">
@@ -6583,7 +6583,7 @@
         <v>5.0</v>
       </c>
       <c r="D427" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="428">
@@ -6594,7 +6594,7 @@
         <v>5.0</v>
       </c>
       <c r="D428" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="429">
@@ -6608,7 +6608,7 @@
         <v>5.0</v>
       </c>
       <c r="D429" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="430">
@@ -6619,7 +6619,7 @@
         <v>5.0</v>
       </c>
       <c r="D430" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="431">
@@ -6633,7 +6633,7 @@
         <v>5.0</v>
       </c>
       <c r="D431" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="432">
@@ -6644,7 +6644,7 @@
         <v>5.0</v>
       </c>
       <c r="D432" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="433">
@@ -6658,7 +6658,7 @@
         <v>5.0</v>
       </c>
       <c r="D433" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="434">
@@ -6669,7 +6669,7 @@
         <v>5.0</v>
       </c>
       <c r="D434" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="435">
@@ -6683,7 +6683,7 @@
         <v>5.0</v>
       </c>
       <c r="D435" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="436">
@@ -6694,7 +6694,7 @@
         <v>5.0</v>
       </c>
       <c r="D436" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="437">
@@ -6708,7 +6708,7 @@
         <v>5.0</v>
       </c>
       <c r="D437" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="438">
@@ -6719,7 +6719,7 @@
         <v>5.0</v>
       </c>
       <c r="D438" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="439">
@@ -6733,7 +6733,7 @@
         <v>5.0</v>
       </c>
       <c r="D439" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="440">
@@ -6744,7 +6744,7 @@
         <v>5.0</v>
       </c>
       <c r="D440" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="441">
@@ -6758,7 +6758,7 @@
         <v>5.0</v>
       </c>
       <c r="D441" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="442">
@@ -6769,7 +6769,7 @@
         <v>5.0</v>
       </c>
       <c r="D442" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="443">
@@ -6783,7 +6783,7 @@
         <v>5.0</v>
       </c>
       <c r="D443" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="444">
@@ -6794,7 +6794,7 @@
         <v>5.0</v>
       </c>
       <c r="D444" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="445">
@@ -6808,7 +6808,7 @@
         <v>5.0</v>
       </c>
       <c r="D445" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="446">
@@ -6819,7 +6819,7 @@
         <v>5.0</v>
       </c>
       <c r="D446" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="447">
@@ -6833,7 +6833,7 @@
         <v>5.0</v>
       </c>
       <c r="D447" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="448">
@@ -6844,7 +6844,7 @@
         <v>5.0</v>
       </c>
       <c r="D448" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="449">
@@ -6858,7 +6858,7 @@
         <v>5.0</v>
       </c>
       <c r="D449" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="450">
@@ -6869,7 +6869,7 @@
         <v>5.0</v>
       </c>
       <c r="D450" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="451">
@@ -6883,7 +6883,7 @@
         <v>5.0</v>
       </c>
       <c r="D451" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="452">
@@ -6894,7 +6894,7 @@
         <v>5.0</v>
       </c>
       <c r="D452" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="453">
@@ -6908,7 +6908,7 @@
         <v>5.0</v>
       </c>
       <c r="D453" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="454">
@@ -6919,7 +6919,7 @@
         <v>5.0</v>
       </c>
       <c r="D454" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="455">
@@ -6933,7 +6933,7 @@
         <v>5.0</v>
       </c>
       <c r="D455" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="456">
@@ -6944,7 +6944,7 @@
         <v>5.0</v>
       </c>
       <c r="D456" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="457">
@@ -6958,7 +6958,7 @@
         <v>5.0</v>
       </c>
       <c r="D457" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="458">
@@ -6969,7 +6969,7 @@
         <v>5.0</v>
       </c>
       <c r="D458" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="459">
@@ -6983,7 +6983,7 @@
         <v>5.0</v>
       </c>
       <c r="D459" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="460">
@@ -6994,7 +6994,7 @@
         <v>5.0</v>
       </c>
       <c r="D460" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="461">
@@ -7008,7 +7008,7 @@
         <v>5.0</v>
       </c>
       <c r="D461" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="462">
@@ -7019,7 +7019,7 @@
         <v>5.0</v>
       </c>
       <c r="D462" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="463">
@@ -7033,7 +7033,7 @@
         <v>5.0</v>
       </c>
       <c r="D463" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="464">
@@ -7044,7 +7044,7 @@
         <v>5.0</v>
       </c>
       <c r="D464" t="n" s="0">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="465">
@@ -7058,7 +7058,7 @@
         <v>5.0</v>
       </c>
       <c r="D465" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="466">
@@ -7069,7 +7069,7 @@
         <v>4.0</v>
       </c>
       <c r="D466" t="n" s="0">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="467">
@@ -7083,7 +7083,7 @@
         <v>4.0</v>
       </c>
       <c r="D467" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="468">
@@ -7094,7 +7094,7 @@
         <v>4.0</v>
       </c>
       <c r="D468" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="469">
@@ -7108,7 +7108,7 @@
         <v>4.0</v>
       </c>
       <c r="D469" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="470">
@@ -7119,7 +7119,7 @@
         <v>4.0</v>
       </c>
       <c r="D470" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="471">
@@ -7133,7 +7133,7 @@
         <v>4.0</v>
       </c>
       <c r="D471" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="472">
@@ -7144,7 +7144,7 @@
         <v>4.0</v>
       </c>
       <c r="D472" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="473">
@@ -7158,7 +7158,7 @@
         <v>4.0</v>
       </c>
       <c r="D473" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="474">
@@ -7169,7 +7169,7 @@
         <v>4.0</v>
       </c>
       <c r="D474" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="475">
@@ -7183,7 +7183,7 @@
         <v>4.0</v>
       </c>
       <c r="D475" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="476">
@@ -7194,7 +7194,7 @@
         <v>4.0</v>
       </c>
       <c r="D476" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="477">
@@ -7208,7 +7208,7 @@
         <v>4.0</v>
       </c>
       <c r="D477" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="478">
@@ -7219,7 +7219,7 @@
         <v>4.0</v>
       </c>
       <c r="D478" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="479">
@@ -7233,7 +7233,7 @@
         <v>4.0</v>
       </c>
       <c r="D479" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="480">
@@ -7244,7 +7244,7 @@
         <v>4.0</v>
       </c>
       <c r="D480" t="n" s="0">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>